<commit_message>
- update todos - checklist einschätzung
</commit_message>
<xml_diff>
--- a/documentation/specification/TourPlanner_Checklist.xlsx
+++ b/documentation/specification/TourPlanner_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wallisch\Nextcloud\Lehre\BIF4-SWEN2\Semester Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36eb05c4c24fd3aa/Dokumente/FH/BIF/2023_SS/SWEN2/swen2-project/documentation/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8312F4AC-50D7-4D69-AB35-7E0D8CB806FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{8312F4AC-50D7-4D69-AB35-7E0D8CB806FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0AA12A0-BACF-4D4C-A8D5-F714115F7963}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14166" windowHeight="12504" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Uses C# or Java</t>
   </si>
@@ -220,6 +231,9 @@
   </si>
   <si>
     <t>Search performs full-text search in Tours, Tour Logs and computed attributes</t>
+  </si>
+  <si>
+    <t>unsere Einschätzung</t>
   </si>
 </sst>
 </file>
@@ -308,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,11 +330,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -654,45 +664,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.1" x14ac:dyDescent="0.85">
       <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -700,7 +710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -708,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -716,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -724,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
@@ -732,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -740,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
@@ -748,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -756,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -764,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
@@ -772,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -780,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -788,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -796,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -804,12 +814,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
@@ -820,379 +830,393 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6"/>
+    <row r="26" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="C29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A33" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="6">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="6">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A35" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="6">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="6">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:3" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="C42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44"/>
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:3" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
+      <c r="C46" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48"/>
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="6">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="6">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="6">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="C52" s="6">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:3" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
+      <c r="C54" s="6">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-    </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B56"/>
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E57" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C59" s="6">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C60" s="6">
+        <v>2</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="6">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-    </row>
-    <row r="66" spans="1:3" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
+      <c r="C63" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A66" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B71" s="9"/>
-      <c r="C71" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B76"/>
       <c r="C76" s="6"/>
     </row>
-    <row r="78" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
@@ -1203,6 +1227,10 @@
       <c r="C78" s="2">
         <f>SUM(C27:C76)</f>
         <v>60</v>
+      </c>
+      <c r="E78" s="2">
+        <f>SUM(E27:E74)</f>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix picture slider bug
</commit_message>
<xml_diff>
--- a/documentation/specification/TourPlanner_Checklist.xlsx
+++ b/documentation/specification/TourPlanner_Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36eb05c4c24fd3aa/Dokumente/FH/BIF/2023_SS/SWEN2/swen2-project/documentation/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{8312F4AC-50D7-4D69-AB35-7E0D8CB806FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B12151CD-799E-44C3-9319-79F1BF2FFAA9}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{8312F4AC-50D7-4D69-AB35-7E0D8CB806FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2B21131-7B1D-4A3A-81BD-EA41FA957AE9}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1128,11 +1128,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A62" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C62" s="6">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="E78" s="2">
         <f>SUM(E27:E74)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>